<commit_message>
Updated the device parameter
updated the device parameter file to fit the recent changes in the file format
</commit_message>
<xml_diff>
--- a/parameters/DeviceParameters_PBDB-2F-Tp.xlsx
+++ b/parameters/DeviceParameters_PBDB-2F-Tp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ma11115\Box\Github_mohammed_azzouzi\DriftFusion_OPV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ma11115_ic_ac_uk/Documents/github_folder/DriftFusionOPV/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7984D9-E01A-4B43-BDAA-9E23FA2BDD1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7D7984D9-E01A-4B43-BDAA-9E23FA2BDD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{735DB690-5F7B-43BC-BB63-370C59E45402}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>